<commit_message>
Inclusão custo de alimentação no orçamento
</commit_message>
<xml_diff>
--- a/PastaDocsAdministrativos/Orcamento.xlsx
+++ b/PastaDocsAdministrativos/Orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Desktop\Exercicio\teste\PastaDocsAdministrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF83C2F-BB36-4305-9E90-7457FD07DD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E8CB86-EA0A-46A3-975C-2161125636A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Previsão Orcamentária - PROJETO EXEMPLO</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Capão</t>
+  </si>
+  <si>
+    <t>Comida</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,6 +414,14 @@
         <v>1028000</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Alterações no orçamento e registrando no log
</commit_message>
<xml_diff>
--- a/PastaDocsAdministrativos/Orcamento.xlsx
+++ b/PastaDocsAdministrativos/Orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Desktop\Exercicio\teste\PastaDocsAdministrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E8CB86-EA0A-46A3-975C-2161125636A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97181641-4839-469B-9FD8-60ED8BDB1F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,7 +376,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,7 +419,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>1000</v>
+        <v>2200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>